<commit_message>
Combine benchmark reports after each simulation
</commit_message>
<xml_diff>
--- a/benchmark/baselines/openml_100.xlsx
+++ b/benchmark/baselines/openml_100.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\autem\benchmark\baselines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EAFEC4F-5612-4363-90EE-C3C7BDE017B2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4F5455-4124-4498-860B-F899E9A75F20}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14040" yWindow="0" windowWidth="15360" windowHeight="10605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="openml_100" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="108">
   <si>
     <t>kr-vs-kp</t>
   </si>
@@ -1202,7 +1202,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1484,7 +1484,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="D9" t="s">
         <v>1</v>
@@ -1999,7 +1999,7 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="D25" t="s">
         <v>1</v>
@@ -3067,7 +3067,7 @@
         <v>60</v>
       </c>
       <c r="C61" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="D61" t="s">
         <v>1</v>
@@ -3709,6 +3709,9 @@
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>82</v>
+      </c>
+      <c r="C83" t="s">
+        <v>94</v>
       </c>
       <c r="D83" t="s">
         <v>1</v>

</xml_diff>